<commit_message>
implemented payment extensibility and cust ui
</commit_message>
<xml_diff>
--- a/data/branch_list.xlsx
+++ b/data/branch_list.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2023S2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\SC2002_OOP_FOMS\FOMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CABAEA2-29CC-4B6E-85CA-8D634B514C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59EA764-7C76-4908-BFA0-EDD912B028BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
   <sheets>
-    <sheet name="staff" sheetId="1" r:id="rId1"/>
+    <sheet name="branch" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$1:$A$88</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">staff!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">branch!$A$1:$A$88</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">branch!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="13">
-  <si>
-    <t>Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>staffQuota</t>
   </si>
   <si>
     <t>NTU</t>
@@ -52,31 +49,46 @@
     <t>JE</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>North spine Plaza</t>
-  </si>
-  <si>
-    <t>Jurong point</t>
-  </si>
-  <si>
-    <t>Jurong east</t>
-  </si>
-  <si>
-    <t>Staff Quota</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>manager</t>
+    <t>477c0c7e-9d46-4202-969d-f3dd1933a575</t>
+  </si>
+  <si>
+    <t>67136f7c-fcd0-45f1-8859-9e3d183faeb3</t>
+  </si>
+  <si>
+    <t>5cc0e578-41b6-4e7d-b6e8-5f287be3e857</t>
+  </si>
+  <si>
+    <t>North Spine Plaza</t>
+  </si>
+  <si>
+    <t>Jurong Point</t>
+  </si>
+  <si>
+    <t>Jurong East</t>
+  </si>
+  <si>
+    <t>AMK</t>
+  </si>
+  <si>
+    <t>Ang Mo Kio</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20e7adc4-0f30-4019-b1d1-cb2a8d998616</t>
+  </si>
+  <si>
+    <t>cccb4419-e7e1-4f63-b0f2-b9af8c6256c6</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>3da2a086-a730-4d99-9d7e-7ea5af4bf172</t>
   </si>
 </sst>
 </file>
@@ -116,13 +128,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="64"/>
-      <name val="Microsoft Sans Serif"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,6 +139,13 @@
       <color rgb="FFFF0000"/>
       <name val="Microsoft Sans Serif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,13 +173,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,310 +494,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="6" width="22.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="5" width="22.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="3"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="8"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="3"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="2"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="2"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="2"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="2"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="2"/>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="2"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="2"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
menu item deletion when branch is closed
</commit_message>
<xml_diff>
--- a/data/branch_list.xlsx
+++ b/data/branch_list.xlsx
@@ -512,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -543,76 +543,65 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
         <v>11</v>
       </c>
-      <c r="D3">
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+      <c r="A7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
@@ -626,20 +615,20 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
+      <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
@@ -660,10 +649,10 @@
       <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
+      <c r="A23" s="4"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
+      <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
@@ -693,10 +682,10 @@
       <c r="A33" s="3"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3"/>
+      <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="A35" s="3"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
@@ -705,10 +694,10 @@
       <c r="A37" s="3"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="3"/>
+      <c r="A38" s="1"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
+      <c r="A39" s="3"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
@@ -738,31 +727,31 @@
       <c r="A48" s="3"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="3"/>
+      <c r="A49" s="7"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="7"/>
+      <c r="A50" s="1"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="1"/>
+      <c r="A51" s="3"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="3"/>
+      <c r="A53" s="1"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="1"/>
+      <c r="A55" s="3"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="3"/>
+      <c r="A56" s="1"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="1"/>
+      <c r="A57" s="3"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
@@ -782,8 +771,8 @@
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" s="3"/>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="2"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
@@ -808,9 +797,6 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>